<commit_message>
unifying outchannel estimation, fixing various remapping schemes
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_nodes.xlsx
+++ b/configurations/experiment_configs_nodes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -405,7 +405,7 @@
     <t xml:space="preserve">/s/fran_storage/predictions/totalseg/LITS-1088</t>
   </si>
   <si>
-    <t xml:space="preserve">remapping</t>
+    <t xml:space="preserve">remapping_imported</t>
   </si>
   <si>
     <t xml:space="preserve">TSL.all</t>
@@ -1029,7 +1029,7 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -1920,8 +1920,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
config adding channels , labels_all functionality
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_nodes.xlsx
+++ b/configurations/experiment_configs_nodes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -408,7 +408,7 @@
     <t xml:space="preserve">remapping_imported</t>
   </si>
   <si>
-    <t xml:space="preserve">TSL.all</t>
+    <t xml:space="preserve">TSL.all,TSL.all</t>
   </si>
   <si>
     <t xml:space="preserve">merge_imported_labels</t>
@@ -1029,7 +1029,7 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -1920,8 +1920,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
setting up a test manager
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_nodes.xlsx
+++ b/configurations/experiment_configs_nodes.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="161">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve">ds_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plan_test</t>
   </si>
   <si>
     <t xml:space="preserve">plan_valid</t>
@@ -1152,64 +1155,64 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,22 +1220,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -1240,7 +1243,7 @@
         <v>47</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>4</v>
@@ -1255,39 +1258,39 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>47</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>4</v>
@@ -1302,22 +1305,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1325,10 +1328,10 @@
         <v>22</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>4</v>
@@ -1343,27 +1346,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="R5" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>4</v>
@@ -1378,23 +1381,23 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I6" s="3" t="n">
         <v>192</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1402,7 +1405,7 @@
         <v>47</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>4</v>
@@ -1417,36 +1420,36 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>50</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>4</v>
@@ -1461,34 +1464,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>50</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I8" s="3" t="n">
         <v>192</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>4</v>
@@ -1503,34 +1506,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>75</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I9" s="3" t="n">
         <v>192</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>4</v>
@@ -1741,16 +1744,16 @@
       <c r="E12" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>192</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,10 +1761,17 @@
         <v>83</v>
       </c>
       <c r="E14" s="1" t="n">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="1" t="n">
         <v>128</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1803,13 +1813,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1820,114 +1830,114 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0.1</v>
@@ -1938,53 +1948,53 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>0</v>
@@ -1993,7 +2003,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>31</v>
@@ -2046,32 +2056,32 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>0</v>
@@ -2080,29 +2090,29 @@
         <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
@@ -2113,13 +2123,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
@@ -2169,12 +2179,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>0</v>
@@ -2182,7 +2192,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>22</v>
@@ -2190,7 +2200,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0</v>
@@ -2201,18 +2211,18 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
@@ -2267,28 +2277,28 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
@@ -2296,28 +2306,28 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>32</v>
@@ -2333,23 +2343,23 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2398,49 +2408,49 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>32</v>
@@ -2456,23 +2466,23 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>32</v>
@@ -2480,23 +2490,23 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2545,28 +2555,28 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
@@ -2574,28 +2584,28 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>32</v>
@@ -2603,10 +2613,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,23 +2629,23 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2684,28 +2694,28 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
@@ -2713,28 +2723,28 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>32</v>
@@ -2742,7 +2752,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>